<commit_message>
Atualizando site, criando novas funcionalidades
</commit_message>
<xml_diff>
--- a/planilhas/coleta_RioDesign_manha.xlsx
+++ b/planilhas/coleta_RioDesign_manha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Endereço</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Complemento</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +461,20 @@
           <t>aa</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intimissimi</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Av</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>